<commit_message>
Centered and Bold Headers
</commit_message>
<xml_diff>
--- a/LokkaL Work Log.xlsx
+++ b/LokkaL Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\AndroidStudioProjects\LokkaL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933EDEB-C840-443C-829F-D36FCCCB94CC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85E842-725B-4B5C-AE09-233F03568E24}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{4B93EF9E-968D-4891-AAA2-27858ECFC76B}"/>
   </bookViews>
@@ -169,8 +169,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,12 +206,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -522,9 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4F3854-BC87-4903-8D21-78D2A2974270}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -534,13 +543,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -986,5 +995,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>